<commit_message>
working on Debugger issues
</commit_message>
<xml_diff>
--- a/Dependencies.xlsx
+++ b/Dependencies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Utils</t>
   </si>
@@ -392,7 +392,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +442,9 @@
         <v>3</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
back to work on Engine/Cores creation
</commit_message>
<xml_diff>
--- a/Dependencies.xlsx
+++ b/Dependencies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Utils</t>
   </si>
@@ -72,14 +72,25 @@
   </si>
   <si>
     <t>Forecaster</t>
+  </si>
+  <si>
+    <t>Destroyer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,8 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,229 +403,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
+      <c r="D8">
+        <v>3</v>
       </c>
       <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started working on cuNN. need to read Topology & Training sections
</commit_message>
<xml_diff>
--- a/Dependencies.xlsx
+++ b/Dependencies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
   <si>
     <t>Utils</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Destroyer</t>
+  </si>
+  <si>
+    <t>cuSVM</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +427,7 @@
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -429,7 +435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -437,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -445,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -453,7 +459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -467,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -484,7 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -504,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -527,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -541,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -561,7 +567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -575,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -586,76 +592,108 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D16">
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
         <v>13</v>
       </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>